<commit_message>
V0.5.0 Added Multiple Data Fields and Field Selection
</commit_message>
<xml_diff>
--- a/SimpleData.xlsx
+++ b/SimpleData.xlsx
@@ -13,22 +13,28 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1711413291" val="1068" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1711413291" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1711413291" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1711413291"/>
+      <pm:revision xmlns:pm="smNativeData" day="1713029752" val="1068" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1713029752" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1713029752" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1713029752"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
   <si>
     <t>Age</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Salary</t>
   </si>
   <si>
     <t>John</t>
@@ -80,7 +86,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1711413291" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1713029752" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -95,7 +101,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1711413291" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1713029752" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -117,7 +123,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1711413291" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1713029752" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -139,7 +145,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1711413291"/>
+          <pm:border xmlns:pm="smNativeData" id="1713029752"/>
         </ext>
       </extLst>
     </border>
@@ -158,7 +164,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1711413291"/>
+          <pm:border xmlns:pm="smNativeData" id="1713029752"/>
         </ext>
       </extLst>
     </border>
@@ -175,7 +181,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1711413291" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1713029752" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -439,99 +445,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="n">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="n">
+        <v>73</v>
+      </c>
+      <c r="D2" t="n">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" t="n">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="n">
+        <v>32</v>
+      </c>
+      <c r="D3" t="n">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="n">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="n">
+        <v>46</v>
+      </c>
+      <c r="D4" t="n">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" t="n">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" t="n">
+        <v>89</v>
+      </c>
+      <c r="D5" t="n">
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="n">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" t="n">
         <v>53</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" t="n">
+        <v>63</v>
+      </c>
+      <c r="D7" t="n">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" t="n">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" t="n">
+        <v>25</v>
+      </c>
+      <c r="D8" t="n">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" t="n">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" t="n">
+        <v>55</v>
+      </c>
+      <c r="D9" t="n">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10" t="n">
         <v>40</v>
+      </c>
+      <c r="C10" t="n">
+        <v>95</v>
+      </c>
+      <c r="D10" t="n">
+        <v>80000</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1711413291" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1713029752" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -540,14 +606,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1711413291" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1711413291" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1713029752" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1713029752" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1711413291" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1713029752" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>